<commit_message>
Update to all files
</commit_message>
<xml_diff>
--- a/tables/funding.xlsx
+++ b/tables/funding.xlsx
@@ -3,26 +3,28 @@
 </file>
 
 <file path=META-INF/manifest.xml><?xml version="1.0" encoding="utf-8"?>
-<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" manifest:version="1.2">
-  <manifest:file-entry manifest:media-type="application/vnd.oasis.opendocument.spreadsheet" manifest:version="1.2" manifest:full-path="/"/>
-  <manifest:file-entry manifest:media-type="" manifest:full-path="Configurations2/accelerator/current.xml"/>
-  <manifest:file-entry manifest:media-type="application/vnd.sun.xml.ui.configuration" manifest:full-path="Configurations2/"/>
-  <manifest:file-entry manifest:media-type="image/png" manifest:full-path="Thumbnails/thumbnail.png"/>
-  <manifest:file-entry manifest:media-type="text/xml" manifest:full-path="content.xml"/>
-  <manifest:file-entry manifest:media-type="text/xml" manifest:full-path="settings.xml"/>
-  <manifest:file-entry manifest:media-type="text/xml" manifest:full-path="styles.xml"/>
-  <manifest:file-entry manifest:media-type="application/rdf+xml" manifest:full-path="manifest.rdf"/>
-  <manifest:file-entry manifest:media-type="text/xml" manifest:full-path="meta.xml"/>
+<manifest:manifest xmlns:manifest="urn:oasis:names:tc:opendocument:xmlns:manifest:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" manifest:version="1.3">
+  <manifest:file-entry manifest:full-path="/" manifest:version="1.3" manifest:media-type="application/vnd.oasis.opendocument.spreadsheet"/>
+  <manifest:file-entry manifest:full-path="Configurations2/accelerator/current.xml" manifest:media-type=""/>
+  <manifest:file-entry manifest:full-path="Configurations2/" manifest:media-type="application/vnd.sun.xml.ui.configuration"/>
+  <manifest:file-entry manifest:full-path="manifest.rdf" manifest:media-type="application/rdf+xml"/>
+  <manifest:file-entry manifest:full-path="styles.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="meta.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="content.xml" manifest:media-type="text/xml"/>
+  <manifest:file-entry manifest:full-path="Thumbnails/thumbnail.png" manifest:media-type="image/png"/>
+  <manifest:file-entry manifest:full-path="settings.xml" manifest:media-type="text/xml"/>
 </manifest:manifest>
 </file>
 
 <file path=content.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-content xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" office:version="1.2">
+<office:document-content xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:scripts/>
   <office:font-face-decls>
     <style:font-face style:name="Arial" svg:font-family="Arial" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Arial1" svg:font-family="Arial" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans Unicode" svg:font-family="'Lucida Sans Unicode'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Tahoma" svg:font-family="Tahoma" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -44,24 +46,27 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="2.5484in"/>
     </style:style>
     <style:style style:name="co6" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="1.95in"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.7382in"/>
     </style:style>
     <style:style style:name="co7" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.672in"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
-      <style:table-row-properties style:row-height="0.1953in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.1917in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro2" style:family="table-row">
-      <style:table-row-properties style:row-height="0.3937in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.3311in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="1.5134in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="1.2638in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro4" style:family="table-row">
+      <style:table-row-properties style:row-height="1.4193in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro5" style:family="table-row">
       <style:table-row-properties style:row-height="3.3335in" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro5" style:family="table-row">
+    <style:style style:name="ro6" style:family="table-row">
       <style:table-row-properties style:row-height="1.4063in" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="PageStyle_5f_Sheet1">
@@ -70,21 +75,21 @@
     <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
       <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom"/>
-      <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce8" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in" style:writing-mode="page"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
       <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in"/>
     </style:style>
     <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom"/>
       <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
     </style:style>
     <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom"/>
@@ -97,6 +102,15 @@
     <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in" style:writing-mode="page"/>
+    </style:style>
+    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Excel_20_Built-in_20_Normal">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom"/>
+      <style:paragraph-properties fo:text-align="end" fo:margin-left="0in" style:writing-mode="page"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
+      <style:paragraph-properties fo:text-align="justify" fo:margin-left="0in"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -106,107 +120,122 @@
       </table:calculation-settings>
       <table:table table:name="Sheet1" table:style-name="ta1" table:print="false">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co4" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co5" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co7" table:number-columns-repeated="1018" table:default-cell-style-name="ce3"/>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
-          <table:table-cell table:style-name="ce1" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce4" table:number-columns-repeated="4"/>
-          <table:table-cell table:number-columns-repeated="1018"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co4" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co5" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co7" table:number-columns-repeated="58" table:default-cell-style-name="ce9"/>
+        <table:table-column table:style-name="co7" table:number-columns-repeated="960" table:default-cell-style-name="ce16"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+            <text:p>A</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+            <text:p>B</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>C</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>D</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>E</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>F</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell table:style-name="ce1" office:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Area title </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Indicator</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Description of the Indicators </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Calculations/measurement/presence/absence</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Primary source of data </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Alternative indicator</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1018"/>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string">
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>PUBLIC SPENDING</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Sources of public funding (at local level)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Number of existing sources of funding available for SE from public donors (exact programmes and funds)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>1) Total annual budget (in euros) - from all available funds (at local level)</text:p>
             <text:p>Or </text:p>
             <text:p>2) Number of existing sources of funding available for SE from public donors (exact programmes and funds)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Governmental site for social economy, local municipality site, sites of ministries</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce2" office:value-type="string">
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>
               Type of other resources and types of non-financial 
               <text:s text:c="2"/>
               donations provided by public entities
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1018"/>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell table:style-name="ce2" office:value-type="string">
-            <text:p>PUBLIC SPENDING</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:covered-table-cell table:style-name="Default"/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Local spending for SE (or SME and StartUps) </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>% of total local budget </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               1) used % of total local budget 
               <text:s/>
               for SE 
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Local municipality office</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell table:number-columns-repeated="1018"/>
+          <table:covered-table-cell table:style-name="ce15"/>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce1" office:value-type="string">
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
             <text:p>PRIVATE INVESTMENT</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Funding institutions</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string">
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Number of private stakeholders providing financial services for SE</text:p>
             <text:p>Percentage of banks that have instruments applicable to SE</text:p>
             <text:p>Types of funding institutions - bank, saving house, etc.</text:p>
-            <text:p>
-              Types of funding instruments - Credit, grants, loans, 
-              <text:s/>
-              angel investors, ventures, etc
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+            <text:p>Types of funding instruments - Credit, grants, loans,  angel investors, ventures, etc</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>
               1) used % of total local budget 
               <text:s/>
@@ -217,52 +246,63 @@
               private funding and investment entities available for social entrepreneurship, including grants, loans, and investments
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Banks, private funds (e.g. Coca cola), business angels, CSR (corporate social responsibility </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>
               Type of other resources and types of non-financial 
               <text:s text:c="2"/>
               donations provided by private entities
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1018"/>
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
         </table:table-row>
         <table:table-row table:style-name="ro5">
-          <table:table-cell table:style-name="ce1" office:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>CHARITABLE GIVING</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Donations for support of SE</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce6" office:value-type="string">
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>
               Existing of crowdfunding platforms available for SEs 
-              <text:s text:c="10"/>
-              <text:s text:c="30"/>
+              <text:s/>
               Donor money, crowdfunding, family money
             </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>1) Total amount of donations received by social enterprises from various sources, such as individuals, corporations, foundations, and government agencies. 2) Number and/or value of grants, sponsorships, or crowdfunding campaigns specifically targeted at supporting social entrepreneurship in the local area.3) Percentage or number of social enterprises that report receiving financial contributions or in-kind donations from the community or other stakeholders.</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce5" office:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Contact the se or find it in the business register (annual report)</text:p>
             <text:p>online research </text:p>
             <text:p>incubators (they should know how much money entrepreneurs have when they come)</text:p>
             <text:p>directly from donators and foundations (register whom they give money to)</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>
               Type of other resources and types of non-financial 
               <text:s text:c="2"/>
               donations provided by private entities
             </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1018"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="42"/>
+          <table:table-cell table:number-columns-repeated="976"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell table:style-name="Default" table:number-columns-repeated="48"/>
+          <table:table-cell table:number-columns-repeated="976"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce7"/>
+          <table:table-cell table:number-columns-repeated="1021"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce7"/>
           <table:table-cell table:number-columns-repeated="1021"/>
@@ -274,39 +314,39 @@
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
       </table:table>
+      <table:named-expressions/>
     </office:spreadsheet>
   </office:body>
 </office:document-content>
 </file>
 
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
+<office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
-    <dc:date>2023-08-09T19:46:37.53</dc:date>
-    <dc:creator>nikola pavlov</dc:creator>
-    <meta:generator>OpenOffice/4.1.14$Win32 OpenOffice.org_project/4114m1$Build-9811</meta:generator>
-    <meta:editing-duration>PT41M4S</meta:editing-duration>
-    <meta:editing-cycles>7</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="29" meta:object-count="0"/>
+    <dc:date>2023-08-11T01:21:05.793000000</dc:date>
+    <meta:generator>LibreOffice/7.0.3.1$Windows_X86_64 LibreOffice_project/d7547858d014d4cf69878db179d326fc3483e082</meta:generator>
+    <meta:editing-duration>PT7H35M10S</meta:editing-duration>
+    <meta:editing-cycles>20</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="34" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
 
 <file path=settings.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" xmlns:ooo="http://openoffice.org/2004/office" office:version="1.2">
+<office:document-settings xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:config="urn:oasis:names:tc:opendocument:xmlns:config:1.0" office:version="1.3">
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
-      <config:config-item config:name="VisibleAreaTop" config:type="int">987</config:config-item>
+      <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">35298</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">17816</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">37433</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">17451</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -317,24 +357,27 @@
               <config:config-item config:name="PositionTop" config:type="int">3</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">65</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">674</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1392</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-          <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+          <config:config-item config:name="ZoomValue" config:type="int">65</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
           <config:config-item config:name="ShowPageBreakPreview" config:type="boolean">false</config:config-item>
           <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
           <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-          <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
+          <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
           <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
           <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
           <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
+          <config:config-item config:name="IsValueHighlightingEnabled" config:type="boolean">false</config:config-item>
           <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
           <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
           <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
@@ -342,12 +385,36 @@
           <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
           <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
           <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
+          <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
         </config:config-item-map-entry>
       </config:config-item-map-indexed>
     </config:config-item-set>
     <config:config-item-set config:name="ooo:configuration-settings">
-      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedComplexScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
+      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
+      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
+      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
+      <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
+      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
+      <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Microsoft Print to PDF</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">GRb+/01pY3Jvc29mdCBQcmludCB0byBQREYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAATWljcm9zb2Z0IFByaW50IFRvIFBERgAAAAAAAAAAAAAWAAEANhUAAAAAAAAIAFZUAAAkbQAAM1ROVwAAAAAKAE0AaQBjAHIAbwBzAG8AZgB0ACAAUAByAGkAbgB0ACAAdABvACAAUABEAEYAAAAAAAAAAAAAAAAAAAAAAAAAAAABBAMG3ABQFAMvAQABAAEA6gpvCGQAAQAPAFgCAgABAFgCAwABAEwAZQB0AHQAZQByAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAABAAAA/////0dJUzQAAAAAAAAAAAAAAABESU5VIgDIACQDLBE/XXt+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAkAAQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAyAAAAFNNVEoAAAAAEAC4AHsAMAA4ADQARgAwADEARgBBAC0ARQA2ADMANAAtADQARAA3ADcALQA4ADMARQBFAC0AMAA3ADQAOAAxADcAQwAwADMANQA4ADEAfQAAAFJFU0RMTABVbmlyZXNETEwAUGFwZXJTaXplAExFVFRFUgBPcmllbnRhdGlvbgBQT1JUUkFJVABSZXNvbHV0aW9uAFJlc09wdGlvbjEAQ29sb3JNb2RlAENvbG9yAAAAAAAAAAAAAAAAAAAsEQAAVjRETQEAAAAAAAAAnApwIhwAAADsAAAAAwAAAPoBTwg05ndNg+4HSBfANYHQAAAATAAAAAMAAAAACAAAAAAAAAAAAAADAAAAAAgAACoAAAAACAAAAwAAAEAAAABWAAAAABAAAEQAbwBjAHUAbQBlAG4AdABVAHMAZQByAFAAYQBzAHMAdwBvAHIAZAAAAEQAbwBjAHUAbQBlAG4AdABPAHcAbgBlAHIAUABhAHMAcwB3AG8AcgBkAAAARABvAGMAdQBtAGUAbgB0AEMAcgB5AHAAdABTAGUAYwB1AHIAaQB0AHkAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24=</config:config-item>
+      <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
       <config:config-item-map-indexed config:name="ForbiddenCharacters">
         <config:config-item-map-entry>
           <config:config-item config:name="Language" config:type="string">en</config:config-item>
@@ -357,42 +424,29 @@
           <config:config-item config:name="EndLine" config:type="string"/>
         </config:config-item-map-entry>
       </config:config-item-map-indexed>
-      <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
+      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
-      <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
-      <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
-      <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">SEC8425196F60C5</config:config-item>
-      <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="IsOutlineSymbolsSet" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
-      <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">rgX+/1NFQzg0MjUxOTZGNjBDNQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU2Ftc3VuZyBNMjY3eCAyODd4IFNlcmllcyBDbGFzcwAWAAEA1AQAAAAAAAAIAFZUAAAkbQAAM1ROVwIACABTAEUAQwA4ADQAMgA1ADEAOQA2AEYANgAwAEMANQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQQDBtwA8ANDtwACAQABAOoKbwhkAAEADwBYAgEAAQBYAgMAAQBMAGUAdAB0AGUAcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAAAAAAAAAAEAAAACAAAAAQAAAP////9HSVM0AAAAAAAAAAAAAAAARElOVSIAeAHUAxwAUX3nQgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAOAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHgBAABTTVRKAAAAABAAaAF7AEQARQBFADUAMgA1AEUAMgAtAEUAQgAyAEIALQA0ADcANgBCAC0AOABDADIAQQAtADMAOABBADQAQQBBADkANQA2ADYAMABFAH0AAABJbnB1dEJpbgBBVVRPAFJFU0RMTABVbmlyZXNETEwAT3JpZW50YXRpb24AUE9SVFJBSVQAQ29sbGF0ZQBPRkYATWVkaWFUeXBlAFByaW50ZXJEZWZhdWx0AEpvYlJldmVyc2VEdXBsZXgAT0ZGAFJlc29sdXRpb24AZHBpXzYwMHg2MDB4MQBQYXBlclNpemUATEVUVEVSAER1cGxleABOT05FAFBhZ2VzUGVyU2hlZXQAMQBQYWdlT3JkZXIARnJvbnRUb0JhY2sAQm9va2xldABPRkYAUGFnZUJvcmRlcgBPRkYAQ29sb3JNb2RlAEdyYXlzY2FsZQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAcAAAAVjRETQEAAAAAAAAAAAAAAAAAAAAAAAAAEgBDT01QQVRfRFVQTEVYX01PREUKAERVUExFWF9PRkY=</config:config-item>
-      <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
-      <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
-      <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="EmbedAsianScriptFonts" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
 </file>
 
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
-<office:document-styles xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" office:version="1.2">
+<office:document-styles xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:rpt="http://openoffice.org/2005/report" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:css3t="http://www.w3.org/TR/css3-text/" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" office:version="1.3">
   <office:font-face-decls>
     <style:font-face style:name="Arial" svg:font-family="Arial" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Calibri" svg:font-family="Calibri" style:font-family-generic="swiss" style:font-pitch="variable"/>
+    <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="Arial1" svg:font-family="Arial" style:font-family-generic="system" style:font-pitch="variable"/>
+    <style:font-face style:name="Lucida Sans" svg:font-family="'Lucida Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Lucida Sans Unicode" svg:font-family="'Lucida Sans Unicode'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Microsoft YaHei" svg:font-family="'Microsoft YaHei'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="Tahoma" svg:font-family="Tahoma" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -405,102 +459,102 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:currency-style style:name="N104P0" style:volatile="true">
+    <number:currency-style style:name="N122P0" style:volatile="true">
       <number:currency-symbol number:language="en" number:country="US">$</number:currency-symbol>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-    </number:currency-style>
-    <number:currency-style style:name="N104">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+    </number:currency-style>
+    <number:currency-style style:name="N122">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
       <number:currency-symbol number:language="en" number:country="US">$</number:currency-symbol>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N104P0"/>
-    </number:currency-style>
-    <number:number-style style:name="N8000" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N122P0"/>
+    </number:currency-style>
+    <number:number-style style:name="N10000" number:language="en" number:country="US">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:currency-style style:name="N8116P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8116" number:language="en" number:country="US">
+    <number:currency-style style:name="N10122P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10122" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8116P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N8117P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8117" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10122P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N10123P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10123" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8117P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N8118P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8118" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10123P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N10125P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10125" number:language="en" number:country="US">
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8118P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N8119P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8119" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10125P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N10126P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10126" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8119P0"/>
-    </number:currency-style>
-    <number:date-style style:name="N8120" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10126P0"/>
+    </number:currency-style>
+    <number:date-style style:name="N10127" number:language="en" number:country="US">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
       <number:text>/</number:text>
       <number:year number:style="long"/>
     </number:date-style>
-    <number:date-style style:name="N8121" number:language="en" number:country="US">
+    <number:date-style style:name="N10128" number:language="en" number:country="US">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N8122" number:language="en" number:country="US">
+    <number:date-style style:name="N10129" number:language="en" number:country="US">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
     </number:date-style>
-    <number:date-style style:name="N8123" number:language="en" number:country="US">
+    <number:date-style style:name="N10130" number:language="en" number:country="US">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:time-style style:name="N8124" number:language="en" number:country="US">
+    <number:time-style style:name="N10131" number:language="en" number:country="US">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N8125" number:language="en" number:country="US">
+    <number:time-style style:name="N10132" number:language="en" number:country="US">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
@@ -509,19 +563,19 @@
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N8126" number:language="en" number:country="US">
+    <number:time-style style:name="N10133" number:language="en" number:country="US">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N8127" number:language="en" number:country="US">
+    <number:time-style style:name="N10134" number:language="en" number:country="US">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:date-style style:name="N8128" number:language="en" number:country="US">
+    <number:date-style style:name="N10135" number:language="en" number:country="US">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
@@ -532,185 +586,230 @@
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:date-style>
-    <number:number-style style:name="N8129P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8129" number:language="en" number:country="US">
+    <number:number-style style:name="N10137P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10137" number:language="en" number:country="US">
       <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8129P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8130P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8130" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10137P0"/>
+    </number:number-style>
+    <number:number-style style:name="N10138P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10138" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8130P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8131P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8131" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10138P0"/>
+    </number:number-style>
+    <number:number-style style:name="N10140P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10140" number:language="en" number:country="US">
       <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8131P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8132P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8132" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10140P0"/>
+    </number:number-style>
+    <number:number-style style:name="N10141P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10141" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8132P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8133P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8133P1" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N10141P0"/>
+    </number:number-style>
+    <number:number-style style:name="N10145P0" style:volatile="true" number:language="en" number:country="US">
+      <number:text> </number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10145P1" style:volatile="true" number:language="en" number:country="US">
       <number:text> (</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N8133P2" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N10145P2" style:volatile="true" number:language="en" number:country="US">
       <number:text> - </number:text>
     </number:number-style>
-    <number:text-style style:name="N8133" number:language="en" number:country="US">
+    <number:text-style style:name="N10145" number:language="en" number:country="US">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8133P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8133P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8133P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N10145P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N10145P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N10145P2"/>
     </number:text-style>
-    <number:currency-style style:name="N8134P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8134P1" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:currency-style style:name="N10148P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10148P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8134P2" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10148P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>- </number:text>
     </number:currency-style>
-    <number:text-style style:name="N8134" number:language="en" number:country="US">
+    <number:text-style style:name="N10148" number:language="en" number:country="US">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8134P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8134P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8134P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N10148P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N10148P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N10148P2"/>
     </number:text-style>
-    <number:number-style style:name="N8135P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8135P1" style:volatile="true" number:language="en" number:country="US">
+    <number:number-style style:name="N10152P0" style:volatile="true" number:language="en" number:country="US">
+      <number:text> </number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N10152P1" style:volatile="true" number:language="en" number:country="US">
       <number:text> (</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N8135P2" style:volatile="true" number:language="en" number:country="US">
-      <number:text> -</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:text-style style:name="N8135" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N10152P2" style:volatile="true" number:language="en" number:country="US">
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:text-style style:name="N10152" number:language="en" number:country="US">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8135P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8135P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8135P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N10152P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N10152P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N10152P2"/>
     </number:text-style>
-    <number:currency-style style:name="N8136P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8136P1" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:currency-style style:name="N10155P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10155P1" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8136P2" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N10155P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N8136" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N10155" number:language="en" number:country="US">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8136P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8136P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8136P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N10155P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N10155P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N10155P2"/>
     </number:text-style>
-    <number:time-style style:name="N8137" number:language="en" number:country="US">
+    <number:time-style style:name="N10156" number:language="en" number:country="US">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N8138" number:language="en" number:country="US" number:truncate-on-overflow="false">
+    <number:time-style style:name="N10157" number:language="en" number:country="US" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N8139" number:language="en" number:country="US">
+    <number:time-style style:name="N10158" number:language="en" number:country="US">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N8140" number:language="en" number:country="US">
-      <number:scientific-number number:decimal-places="1" number:min-integer-digits="3" number:min-exponent-digits="1"/>
+    <number:number-style style:name="N10159" number:language="en" number:country="US">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="3" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
-      <style:text-properties style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial1"/>
-    </style:style>
-    <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
-      <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold"/>
-    </style:style>
-    <style:style style:name="Result2" style:family="table-cell" style:parent-style-name="Result" style:data-style-name="N104"/>
+      <style:text-properties style:font-name-asian="Microsoft YaHei" style:font-family-asian="'Microsoft YaHei'" style:font-family-generic-asian="system" style:font-pitch-asian="variable" style:font-name-complex="Arial1" style:font-family-complex="Arial" style:font-family-generic-complex="system" style:font-pitch-complex="variable"/>
+    </style:style>
     <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
       <style:paragraph-properties fo:text-align="center"/>
       <style:text-properties fo:font-size="16pt" fo:font-style="italic" fo:font-weight="bold"/>
     </style:style>
+    <style:style style:name="Heading_20_1" style:display-name="Heading 1" style:family="table-cell" style:parent-style-name="Heading">
+      <style:text-properties fo:color="#000000" fo:font-size="18pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Heading_20_2" style:display-name="Heading 2" style:family="table-cell" style:parent-style-name="Heading">
+      <style:text-properties fo:color="#000000" fo:font-size="12pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Text" style:family="table-cell" style:parent-style-name="Default"/>
+    <style:style style:name="Note" style:family="table-cell" style:parent-style-name="Text">
+      <style:table-cell-properties fo:background-color="#ffffcc" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" fo:border="0.74pt solid #808080"/>
+      <style:text-properties fo:color="#333333" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Footnote" style:family="table-cell" style:parent-style-name="Text">
+      <style:text-properties fo:color="#808080" fo:font-size="10pt" fo:font-style="italic" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Hyperlink" style:family="table-cell" style:parent-style-name="Text">
+      <style:text-properties fo:color="#0000ee" fo:font-size="10pt" fo:font-style="normal" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="#0000ee" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Status" style:family="table-cell" style:parent-style-name="Default"/>
+    <style:style style:name="Good" style:family="table-cell" style:parent-style-name="Status">
+      <style:table-cell-properties fo:background-color="#ccffcc"/>
+      <style:text-properties fo:color="#006600" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Neutral" style:family="table-cell" style:parent-style-name="Status">
+      <style:table-cell-properties fo:background-color="#ffffcc"/>
+      <style:text-properties fo:color="#996600" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Bad" style:family="table-cell" style:parent-style-name="Status">
+      <style:table-cell-properties fo:background-color="#ffcccc"/>
+      <style:text-properties fo:color="#cc0000" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Warning" style:family="table-cell" style:parent-style-name="Status">
+      <style:text-properties fo:color="#cc0000" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Error" style:family="table-cell" style:parent-style-name="Status">
+      <style:table-cell-properties fo:background-color="#cc0000"/>
+      <style:text-properties fo:color="#ffffff" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="bold"/>
+    </style:style>
+    <style:style style:name="Accent" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="bold"/>
+    </style:style>
+    <style:style style:name="Accent_20_1" style:display-name="Accent 1" style:family="table-cell" style:parent-style-name="Accent">
+      <style:table-cell-properties fo:background-color="#000000"/>
+      <style:text-properties fo:color="#ffffff" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Accent_20_2" style:display-name="Accent 2" style:family="table-cell" style:parent-style-name="Accent">
+      <style:table-cell-properties fo:background-color="#808080"/>
+      <style:text-properties fo:color="#ffffff" fo:font-size="10pt" fo:font-style="normal" fo:font-weight="normal"/>
+    </style:style>
+    <style:style style:name="Accent_20_3" style:display-name="Accent 3" style:family="table-cell" style:parent-style-name="Accent">
+      <style:table-cell-properties fo:background-color="#dddddd"/>
+    </style:style>
+    <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold"/>
+    </style:style>
+    <style:style style:name="Result2" style:family="table-cell" style:parent-style-name="Result" style:data-style-name="N122"/>
     <style:style style:name="Heading1" style:family="table-cell" style:parent-style-name="Heading">
       <style:table-cell-properties style:rotation-angle="90"/>
     </style:style>
-    <style:style style:name="Excel_20_Built-in_20_Normal" style:display-name="Excel Built-in Normal" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N8000">
+    <style:style style:name="Excel_20_Built-in_20_Normal" style:display-name="Excel Built-in Normal" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N10000">
       <style:table-cell-properties style:cell-protect="protected" style:print-content="true" style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="value-type" style:repeat-content="false" fo:background-color="transparent" fo:wrap-option="no-wrap" fo:border="none" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom"/>
       <style:paragraph-properties fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-family="Calibri" style:font-family-generic="swiss" style:font-pitch="variable" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri" style:font-family-complex="Calibri" style:font-family-generic-complex="swiss" style:font-pitch-complex="variable" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
   </office:styles>
   <office:automatic-styles>
@@ -726,12 +825,12 @@
     <style:page-layout style:name="Mpm2">
       <style:page-layout-properties style:writing-mode="lr-tb"/>
       <style:header-style>
-        <style:header-footer-properties fo:min-height="0.2957in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-bottom="0.0984in" fo:border="0.0346in solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.2957in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-bottom="0.0984in" fo:border="2.49pt solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:header-style>
       <style:footer-style>
-        <style:header-footer-properties fo:min-height="0.2957in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-top="0.0984in" fo:border="0.0346in solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
+        <style:header-footer-properties fo:min-height="0.2957in" fo:margin-left="0in" fo:margin-right="0in" fo:margin-top="0.0984in" fo:border="2.49pt solid #000000" fo:padding="0.0071in" fo:background-color="#c0c0c0">
           <style:background-image/>
         </style:header-footer-properties>
       </style:footer-style>
@@ -767,16 +866,17 @@
         <style:region-left>
           <text:p>
             <text:sheet-name>???</text:sheet-name>
-             (
+            <text:s/>
+            (
             <text:title>???</text:title>
             )
           </text:p>
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2023-08-09">08/09/2023</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2023-08-11">00/00/0000</text:date>
             , 
-            <text:time>19:46:37</text:time>
+            <text:time style:data-style-name="N2" text:time-value="18:40:11.831000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>
@@ -785,7 +885,8 @@
         <text:p>
           Page 
           <text:page-number>1</text:page-number>
-           / 
+          <text:s/>
+          / 
           <text:page-count>99</text:page-count>
         </text:p>
       </style:footer>

</xml_diff>